<commit_message>
Update chart date ranges
... but still can't get axes to display correctly
</commit_message>
<xml_diff>
--- a/data/covid-stats.xlsx
+++ b/data/covid-stats.xlsx
@@ -503,10 +503,10 @@
           </c:tx>
           <c:cat>
             <c:numRef>
-              <c:f>Austria!$A$6:$A$30</c:f>
+              <c:f>Austria!$A$6:$A$33</c:f>
               <c:numCache>
                 <c:formatCode>dd\-mmm</c:formatCode>
-                <c:ptCount val="25"/>
+                <c:ptCount val="28"/>
                 <c:pt idx="0">
                   <c:v>43899</c:v>
                 </c:pt>
@@ -581,16 +581,25 @@
                 </c:pt>
                 <c:pt idx="24">
                   <c:v>43923</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>43924</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>43925</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>43926</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Austria!$G$6:$G$30</c:f>
+              <c:f>Austria!$G$6:$G$33</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="25"/>
+                <c:ptCount val="28"/>
                 <c:pt idx="0">
                   <c:v>131</c:v>
                 </c:pt>
@@ -665,6 +674,15 @@
                 </c:pt>
                 <c:pt idx="24">
                   <c:v>10967</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -672,8 +690,8 @@
         </c:ser>
         <c:gapWidth val="75"/>
         <c:overlap val="-25"/>
-        <c:axId val="195645824"/>
-        <c:axId val="195639936"/>
+        <c:axId val="193679744"/>
+        <c:axId val="193677952"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -766,10 +784,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Austria!$J$6:$J$30</c:f>
+              <c:f>Austria!$J$6:$J$33</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
-                <c:ptCount val="25"/>
+                <c:ptCount val="28"/>
                 <c:pt idx="5">
                   <c:v>0.38083321236080414</c:v>
                 </c:pt>
@@ -836,11 +854,11 @@
           <c:smooth val="1"/>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="195612032"/>
-        <c:axId val="195638400"/>
+        <c:axId val="193645952"/>
+        <c:axId val="193676416"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="195612032"/>
+        <c:axId val="193645952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -858,13 +876,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="195638400"/>
+        <c:crossAx val="193676416"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="195638400"/>
+        <c:axId val="193676416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -878,24 +896,24 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="195612032"/>
+        <c:crossAx val="193645952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="195639936"/>
+        <c:axId val="193677952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="r"/>
         <c:numFmt formatCode="#,##0" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="195645824"/>
+        <c:crossAx val="193679744"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:dateAx>
-        <c:axId val="195645824"/>
+        <c:axId val="193679744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -903,7 +921,7 @@
         <c:axPos val="b"/>
         <c:numFmt formatCode="dd\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="195639936"/>
+        <c:crossAx val="193677952"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
@@ -918,7 +936,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000233" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000233" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000244" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000244" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
   <c:userShapes r:id="rId1"/>
@@ -1178,25 +1196,25 @@
         </c:ser>
         <c:gapWidth val="75"/>
         <c:overlap val="-25"/>
-        <c:axId val="198427392"/>
-        <c:axId val="198428928"/>
+        <c:axId val="195318528"/>
+        <c:axId val="195320064"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="198427392"/>
+        <c:axId val="195318528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="198428928"/>
+        <c:crossAx val="195320064"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="198428928"/>
+        <c:axId val="195320064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1210,7 +1228,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="198427392"/>
+        <c:crossAx val="195318528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1219,7 +1237,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000278" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000278" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000289" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000289" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1265,10 +1283,10 @@
           </c:tx>
           <c:cat>
             <c:numRef>
-              <c:f>Italy!$A$6:$A$42</c:f>
+              <c:f>Italy!$A$6:$A$47</c:f>
               <c:numCache>
                 <c:formatCode>dd\-mmm</c:formatCode>
-                <c:ptCount val="37"/>
+                <c:ptCount val="42"/>
                 <c:pt idx="0">
                   <c:v>43885</c:v>
                 </c:pt>
@@ -1379,16 +1397,31 @@
                 </c:pt>
                 <c:pt idx="36">
                   <c:v>43921</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>43922</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>43923</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>43924</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>43925</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>43926</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Italy!$G$6:$G$42</c:f>
+              <c:f>Italy!$G$6:$G$47</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="37"/>
+                <c:ptCount val="42"/>
                 <c:pt idx="0">
                   <c:v>229</c:v>
                 </c:pt>
@@ -1499,6 +1532,21 @@
                 </c:pt>
                 <c:pt idx="36">
                   <c:v>105972</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>110574</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1506,8 +1554,8 @@
         </c:ser>
         <c:gapWidth val="75"/>
         <c:overlap val="-25"/>
-        <c:axId val="198571520"/>
-        <c:axId val="198569984"/>
+        <c:axId val="195491328"/>
+        <c:axId val="195489792"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -1642,10 +1690,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Italy!$J$6:$J$42</c:f>
+              <c:f>Italy!$J$6:$J$47</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
-                <c:ptCount val="37"/>
+                <c:ptCount val="42"/>
                 <c:pt idx="4">
                   <c:v>0.32790068162329405</c:v>
                 </c:pt>
@@ -1744,6 +1792,9 @@
                 </c:pt>
                 <c:pt idx="36">
                   <c:v>5.6507163525775582E-2</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>5.0394676803661699E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1751,11 +1802,11 @@
           <c:smooth val="1"/>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="198558464"/>
-        <c:axId val="198560000"/>
+        <c:axId val="195478272"/>
+        <c:axId val="195479808"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="198558464"/>
+        <c:axId val="195478272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1763,13 +1814,13 @@
         <c:numFmt formatCode="d/m" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="198560000"/>
+        <c:crossAx val="195479808"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="198560000"/>
+        <c:axId val="195479808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1783,24 +1834,24 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="198558464"/>
+        <c:crossAx val="195478272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="198569984"/>
+        <c:axId val="195489792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="r"/>
         <c:numFmt formatCode="#,##0" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="198571520"/>
+        <c:crossAx val="195491328"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:dateAx>
-        <c:axId val="198571520"/>
+        <c:axId val="195491328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1808,7 +1859,7 @@
         <c:axPos val="b"/>
         <c:numFmt formatCode="dd\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="198569984"/>
+        <c:crossAx val="195489792"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
@@ -1823,7 +1874,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000255" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000255" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000266" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000266" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
   <c:userShapes r:id="rId1"/>
@@ -2134,25 +2185,25 @@
         </c:ser>
         <c:gapWidth val="75"/>
         <c:overlap val="-25"/>
-        <c:axId val="198604288"/>
-        <c:axId val="198605824"/>
+        <c:axId val="195585536"/>
+        <c:axId val="195587072"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="198604288"/>
+        <c:axId val="195585536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="198605824"/>
+        <c:crossAx val="195587072"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="198605824"/>
+        <c:axId val="195587072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2166,7 +2217,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="198604288"/>
+        <c:crossAx val="195585536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2175,7 +2226,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000233" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000233" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000244" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000244" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2482,25 +2533,25 @@
         </c:ser>
         <c:gapWidth val="75"/>
         <c:overlap val="-25"/>
-        <c:axId val="198625920"/>
-        <c:axId val="198631808"/>
+        <c:axId val="195615360"/>
+        <c:axId val="196157824"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="198625920"/>
+        <c:axId val="195615360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="198631808"/>
+        <c:crossAx val="196157824"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="198631808"/>
+        <c:axId val="196157824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2514,7 +2565,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="198625920"/>
+        <c:crossAx val="195615360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2523,7 +2574,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000255" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000255" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000266" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000266" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2569,10 +2620,10 @@
           </c:tx>
           <c:cat>
             <c:numRef>
-              <c:f>Italy!$A$6:$A$39</c:f>
+              <c:f>Italy!$A$6:$A$47</c:f>
               <c:numCache>
                 <c:formatCode>dd\-mmm</c:formatCode>
-                <c:ptCount val="34"/>
+                <c:ptCount val="42"/>
                 <c:pt idx="0">
                   <c:v>43885</c:v>
                 </c:pt>
@@ -2674,16 +2725,40 @@
                 </c:pt>
                 <c:pt idx="33">
                   <c:v>43918</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>43919</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>43920</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>43921</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>43922</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>43923</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>43924</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>43925</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>43926</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Italy!$L$6:$L$39</c:f>
+              <c:f>Italy!$L$6:$L$47</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="34"/>
+                <c:ptCount val="42"/>
                 <c:pt idx="0">
                   <c:v>7</c:v>
                 </c:pt>
@@ -2785,6 +2860,30 @@
                 </c:pt>
                 <c:pt idx="33">
                   <c:v>10023</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>10779</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>11591</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>12428</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>13155</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2792,8 +2891,8 @@
         </c:ser>
         <c:gapWidth val="75"/>
         <c:overlap val="-25"/>
-        <c:axId val="198937600"/>
-        <c:axId val="198936064"/>
+        <c:axId val="196189184"/>
+        <c:axId val="196187648"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -2928,10 +3027,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Italy!$O$6:$O$39</c:f>
+              <c:f>Italy!$O$6:$O$47</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
-                <c:ptCount val="34"/>
+                <c:ptCount val="42"/>
                 <c:pt idx="4">
                   <c:v>0.25610644257703086</c:v>
                 </c:pt>
@@ -3021,6 +3120,18 @@
                 </c:pt>
                 <c:pt idx="33">
                   <c:v>0.1053296440075961</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>9.5962092781701619E-2</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>9.0999099952427581E-2</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>8.7795064797732136E-2</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>7.5758997059809111E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3028,11 +3139,11 @@
           <c:smooth val="1"/>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="198928640"/>
-        <c:axId val="198934528"/>
+        <c:axId val="196180224"/>
+        <c:axId val="196186112"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="198928640"/>
+        <c:axId val="196180224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3040,13 +3151,13 @@
         <c:numFmt formatCode="d/m" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="198934528"/>
+        <c:crossAx val="196186112"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="198934528"/>
+        <c:axId val="196186112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3060,24 +3171,24 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="198928640"/>
+        <c:crossAx val="196180224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="198936064"/>
+        <c:axId val="196187648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="r"/>
         <c:numFmt formatCode="#,##0" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="198937600"/>
+        <c:crossAx val="196189184"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:dateAx>
-        <c:axId val="198937600"/>
+        <c:axId val="196189184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3085,7 +3196,7 @@
         <c:axPos val="b"/>
         <c:numFmt formatCode="dd\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="198936064"/>
+        <c:crossAx val="196187648"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
@@ -3100,7 +3211,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000255" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000255" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000266" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000266" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3410,25 +3521,25 @@
         </c:ser>
         <c:gapWidth val="75"/>
         <c:overlap val="-25"/>
-        <c:axId val="198949888"/>
-        <c:axId val="198972160"/>
+        <c:axId val="196205568"/>
+        <c:axId val="196227840"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="198949888"/>
+        <c:axId val="196205568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="198972160"/>
+        <c:crossAx val="196227840"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="198972160"/>
+        <c:axId val="196227840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3442,7 +3553,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="198949888"/>
+        <c:crossAx val="196205568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3451,7 +3562,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000278" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000278" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000289" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000289" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3677,25 +3788,25 @@
         </c:ser>
         <c:gapWidth val="75"/>
         <c:overlap val="-25"/>
-        <c:axId val="195652992"/>
-        <c:axId val="195589248"/>
+        <c:axId val="193686912"/>
+        <c:axId val="193623168"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="195652992"/>
+        <c:axId val="193686912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="195589248"/>
+        <c:crossAx val="193623168"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="195589248"/>
+        <c:axId val="193623168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3709,7 +3820,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="195652992"/>
+        <c:crossAx val="193686912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3718,7 +3829,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000211" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000211" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000222" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000222" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3947,25 +4058,25 @@
         </c:ser>
         <c:gapWidth val="75"/>
         <c:overlap val="-25"/>
-        <c:axId val="196088192"/>
-        <c:axId val="196089728"/>
+        <c:axId val="193732992"/>
+        <c:axId val="193734528"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="196088192"/>
+        <c:axId val="193732992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="196089728"/>
+        <c:crossAx val="193734528"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="196089728"/>
+        <c:axId val="193734528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3979,7 +4090,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="196088192"/>
+        <c:crossAx val="193732992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3988,7 +4099,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000233" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000233" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000244" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000244" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4034,10 +4145,10 @@
           </c:tx>
           <c:cat>
             <c:numRef>
-              <c:f>Austria!$A$6:$A$30</c:f>
+              <c:f>Austria!$A$6:$A$33</c:f>
               <c:numCache>
                 <c:formatCode>dd\-mmm</c:formatCode>
-                <c:ptCount val="25"/>
+                <c:ptCount val="28"/>
                 <c:pt idx="0">
                   <c:v>43899</c:v>
                 </c:pt>
@@ -4112,16 +4223,25 @@
                 </c:pt>
                 <c:pt idx="24">
                   <c:v>43923</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>43924</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>43925</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>43926</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Austria!$L$6:$L$30</c:f>
+              <c:f>Austria!$L$6:$L$33</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="25"/>
+                <c:ptCount val="28"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -4196,6 +4316,15 @@
                 </c:pt>
                 <c:pt idx="24">
                   <c:v>158</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4203,8 +4332,8 @@
         </c:ser>
         <c:gapWidth val="75"/>
         <c:overlap val="-25"/>
-        <c:axId val="196150784"/>
-        <c:axId val="196149248"/>
+        <c:axId val="194057728"/>
+        <c:axId val="194056192"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -4297,10 +4426,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Austria!$O$6:$O$30</c:f>
+              <c:f>Austria!$O$6:$O$33</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
-                <c:ptCount val="25"/>
+                <c:ptCount val="28"/>
                 <c:pt idx="7">
                   <c:v>0.6</c:v>
                 </c:pt>
@@ -4361,11 +4490,11 @@
           <c:smooth val="1"/>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="196137728"/>
-        <c:axId val="196139264"/>
+        <c:axId val="193786624"/>
+        <c:axId val="193788160"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="196137728"/>
+        <c:axId val="193786624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4383,13 +4512,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="196139264"/>
+        <c:crossAx val="193788160"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="196139264"/>
+        <c:axId val="193788160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4403,24 +4532,24 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="196137728"/>
+        <c:crossAx val="193786624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="196149248"/>
+        <c:axId val="194056192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="r"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="196150784"/>
+        <c:crossAx val="194057728"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:dateAx>
-        <c:axId val="196150784"/>
+        <c:axId val="194057728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4428,7 +4557,7 @@
         <c:axPos val="b"/>
         <c:numFmt formatCode="dd\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="196149248"/>
+        <c:crossAx val="194056192"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
@@ -4443,7 +4572,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000233" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000233" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000244" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000244" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4669,25 +4798,25 @@
         </c:ser>
         <c:gapWidth val="75"/>
         <c:overlap val="-25"/>
-        <c:axId val="196178304"/>
-        <c:axId val="196179840"/>
+        <c:axId val="194081152"/>
+        <c:axId val="194082688"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="196178304"/>
+        <c:axId val="194081152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="196179840"/>
+        <c:crossAx val="194082688"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="196179840"/>
+        <c:axId val="194082688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4701,7 +4830,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="196178304"/>
+        <c:crossAx val="194081152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4710,7 +4839,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000255" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000255" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000266" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000266" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4756,10 +4885,10 @@
           </c:tx>
           <c:cat>
             <c:numRef>
-              <c:f>UK!$A$6:$A$35</c:f>
+              <c:f>UK!$A$6:$A$38</c:f>
               <c:numCache>
                 <c:formatCode>dd\-mmm</c:formatCode>
-                <c:ptCount val="30"/>
+                <c:ptCount val="33"/>
                 <c:pt idx="0">
                   <c:v>43894</c:v>
                 </c:pt>
@@ -4849,16 +4978,25 @@
                 </c:pt>
                 <c:pt idx="29">
                   <c:v>43923</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>43924</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>43925</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>43926</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>UK!$G$6:$G$35</c:f>
+              <c:f>UK!$G$6:$G$38</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="30"/>
+                <c:ptCount val="33"/>
                 <c:pt idx="0">
                   <c:v>85</c:v>
                 </c:pt>
@@ -4948,6 +5086,15 @@
                 </c:pt>
                 <c:pt idx="29">
                   <c:v>33718</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4955,8 +5102,8 @@
         </c:ser>
         <c:gapWidth val="75"/>
         <c:overlap val="-25"/>
-        <c:axId val="196818816"/>
-        <c:axId val="196817280"/>
+        <c:axId val="195213184"/>
+        <c:axId val="195211648"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -5067,10 +5214,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>UK!$J$6:$J$35</c:f>
+              <c:f>UK!$J$6:$J$38</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
-                <c:ptCount val="30"/>
+                <c:ptCount val="33"/>
                 <c:pt idx="5">
                   <c:v>0.30704061121415749</c:v>
                 </c:pt>
@@ -5152,11 +5299,11 @@
           <c:smooth val="1"/>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="196809856"/>
-        <c:axId val="196811392"/>
+        <c:axId val="195204224"/>
+        <c:axId val="195205760"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="196809856"/>
+        <c:axId val="195204224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5174,13 +5321,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="196811392"/>
+        <c:crossAx val="195205760"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="196811392"/>
+        <c:axId val="195205760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5194,24 +5341,24 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="196809856"/>
+        <c:crossAx val="195204224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="196817280"/>
+        <c:axId val="195211648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="r"/>
         <c:numFmt formatCode="#,##0" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="196818816"/>
+        <c:crossAx val="195213184"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:dateAx>
-        <c:axId val="196818816"/>
+        <c:axId val="195213184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5219,7 +5366,7 @@
         <c:axPos val="b"/>
         <c:numFmt formatCode="dd\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="196817280"/>
+        <c:crossAx val="195211648"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
@@ -5234,7 +5381,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000255" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000255" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000266" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000266" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
   <c:userShapes r:id="rId1"/>
@@ -5491,25 +5638,25 @@
         </c:ser>
         <c:gapWidth val="75"/>
         <c:overlap val="-25"/>
-        <c:axId val="196828160"/>
-        <c:axId val="197273472"/>
+        <c:axId val="195222528"/>
+        <c:axId val="195405696"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="196828160"/>
+        <c:axId val="195222528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="197273472"/>
+        <c:crossAx val="195405696"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="197273472"/>
+        <c:axId val="195405696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5523,7 +5670,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="196828160"/>
+        <c:crossAx val="195222528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5532,7 +5679,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000233" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000233" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000244" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000244" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -5788,25 +5935,25 @@
         </c:ser>
         <c:gapWidth val="75"/>
         <c:overlap val="-25"/>
-        <c:axId val="197292800"/>
-        <c:axId val="197294336"/>
+        <c:axId val="194867968"/>
+        <c:axId val="194869504"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="197292800"/>
+        <c:axId val="194867968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="197294336"/>
+        <c:crossAx val="194869504"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="197294336"/>
+        <c:axId val="194869504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5820,7 +5967,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="197292800"/>
+        <c:crossAx val="194867968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5829,7 +5976,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000255" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000255" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000266" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000266" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -5875,10 +6022,10 @@
           </c:tx>
           <c:cat>
             <c:numRef>
-              <c:f>UK!$A$11:$A$35</c:f>
+              <c:f>UK!$A$11:$A$38</c:f>
               <c:numCache>
                 <c:formatCode>dd\-mmm</c:formatCode>
-                <c:ptCount val="25"/>
+                <c:ptCount val="28"/>
                 <c:pt idx="0">
                   <c:v>43899</c:v>
                 </c:pt>
@@ -5953,16 +6100,25 @@
                 </c:pt>
                 <c:pt idx="24">
                   <c:v>43923</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>43924</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>43925</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>43926</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>UK!$L$11:$L$35</c:f>
+              <c:f>UK!$L$11:$L$38</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="25"/>
+                <c:ptCount val="28"/>
                 <c:pt idx="0">
                   <c:v>5</c:v>
                 </c:pt>
@@ -6037,6 +6193,15 @@
                 </c:pt>
                 <c:pt idx="24">
                   <c:v>2921</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6044,8 +6209,8 @@
         </c:ser>
         <c:gapWidth val="75"/>
         <c:overlap val="-25"/>
-        <c:axId val="198408448"/>
-        <c:axId val="198406912"/>
+        <c:axId val="195299584"/>
+        <c:axId val="195298048"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -6138,10 +6303,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>UK!$O$11:$O$35</c:f>
+              <c:f>UK!$O$11:$O$38</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
-                <c:ptCount val="25"/>
+                <c:ptCount val="28"/>
                 <c:pt idx="0">
                   <c:v>0.5</c:v>
                 </c:pt>
@@ -6223,11 +6388,11 @@
           <c:smooth val="1"/>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="197305856"/>
-        <c:axId val="197307392"/>
+        <c:axId val="194848256"/>
+        <c:axId val="194849792"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="197305856"/>
+        <c:axId val="194848256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6245,13 +6410,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="197307392"/>
+        <c:crossAx val="194849792"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="197307392"/>
+        <c:axId val="194849792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6265,24 +6430,24 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="197305856"/>
+        <c:crossAx val="194848256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="198406912"/>
+        <c:axId val="195298048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="r"/>
         <c:numFmt formatCode="#,##0" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="198408448"/>
+        <c:crossAx val="195299584"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:dateAx>
-        <c:axId val="198408448"/>
+        <c:axId val="195299584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6290,7 +6455,7 @@
         <c:axPos val="b"/>
         <c:numFmt formatCode="dd\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="198406912"/>
+        <c:crossAx val="195298048"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
@@ -6305,7 +6470,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000255" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000255" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000266" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000266" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -6551,12 +6716,12 @@
 <c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.30706</cdr:x>
-      <cdr:y>0.7023</cdr:y>
+      <cdr:x>0.27961</cdr:x>
+      <cdr:y>0.69972</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.32336</cdr:x>
-      <cdr:y>0.86667</cdr:y>
+      <cdr:x>0.29591</cdr:x>
+      <cdr:y>0.86409</cdr:y>
     </cdr:to>
     <cdr:sp macro="" textlink="">
       <cdr:nvSpPr>
@@ -6565,8 +6730,8 @@
       </cdr:nvSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="2344459" y="2488460"/>
-          <a:ext cx="124455" cy="582412"/>
+          <a:off x="2134927" y="2580614"/>
+          <a:ext cx="124454" cy="606209"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <a:avLst/>
@@ -6768,12 +6933,12 @@
 <c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.55089</cdr:x>
-      <cdr:y>0.66882</cdr:y>
+      <cdr:x>0.42739</cdr:x>
+      <cdr:y>0.69345</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.57085</cdr:x>
-      <cdr:y>0.7957</cdr:y>
+      <cdr:x>0.44735</cdr:x>
+      <cdr:y>0.82033</cdr:y>
     </cdr:to>
     <cdr:sp macro="" textlink="">
       <cdr:nvSpPr>
@@ -6782,8 +6947,8 @@
       </cdr:nvSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="4206204" y="2369837"/>
-          <a:ext cx="152399" cy="449574"/>
+          <a:off x="3263202" y="3218013"/>
+          <a:ext cx="152400" cy="588797"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <a:avLst/>
@@ -7031,12 +7196,12 @@
 <c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.3869</cdr:x>
-      <cdr:y>0.73226</cdr:y>
+      <cdr:x>0.34324</cdr:x>
+      <cdr:y>0.73376</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.4032</cdr:x>
-      <cdr:y>0.89663</cdr:y>
+      <cdr:x>0.35954</cdr:x>
+      <cdr:y>0.89813</cdr:y>
     </cdr:to>
     <cdr:sp macro="" textlink="">
       <cdr:nvSpPr>
@@ -7045,8 +7210,8 @@
       </cdr:nvSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="2954046" y="4469452"/>
-          <a:ext cx="124454" cy="1003252"/>
+          <a:off x="2620699" y="4663096"/>
+          <a:ext cx="124455" cy="1044584"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <a:avLst/>
@@ -7376,7 +7541,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H125"/>
   <sheetViews>
-    <sheetView topLeftCell="A76" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="E117" sqref="E117"/>
     </sheetView>
   </sheetViews>
@@ -9241,7 +9406,7 @@
   <dimension ref="A1:P34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B45" sqref="B45"/>
+      <selection activeCell="AE47" sqref="AE47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -12290,7 +12455,7 @@
   <dimension ref="A1:P47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L51" sqref="L51"/>
+      <selection activeCell="AH31" sqref="AH31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Adjust Daily Test chart for Austria
</commit_message>
<xml_diff>
--- a/data/covid-stats.xlsx
+++ b/data/covid-stats.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="60" windowWidth="31620" windowHeight="12450" activeTab="1"/>
+    <workbookView xWindow="396" yWindow="60" windowWidth="31620" windowHeight="12456" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="6" r:id="rId1"/>
@@ -690,8 +690,8 @@
         </c:ser>
         <c:gapWidth val="75"/>
         <c:overlap val="-25"/>
-        <c:axId val="193679744"/>
-        <c:axId val="193677952"/>
+        <c:axId val="183059968"/>
+        <c:axId val="183058432"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -854,11 +854,11 @@
           <c:smooth val="1"/>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="193645952"/>
-        <c:axId val="193676416"/>
+        <c:axId val="184345344"/>
+        <c:axId val="184346880"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="193645952"/>
+        <c:axId val="184345344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -876,13 +876,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="193676416"/>
+        <c:crossAx val="184346880"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="193676416"/>
+        <c:axId val="184346880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -896,24 +896,24 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="193645952"/>
+        <c:crossAx val="184345344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="193677952"/>
+        <c:axId val="183058432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="r"/>
         <c:numFmt formatCode="#,##0" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="193679744"/>
+        <c:crossAx val="183059968"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:dateAx>
-        <c:axId val="193679744"/>
+        <c:axId val="183059968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -921,7 +921,7 @@
         <c:axPos val="b"/>
         <c:numFmt formatCode="dd\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="193677952"/>
+        <c:crossAx val="183058432"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
@@ -936,7 +936,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000244" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000244" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000255" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000255" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
   <c:userShapes r:id="rId1"/>
@@ -1196,25 +1196,25 @@
         </c:ser>
         <c:gapWidth val="75"/>
         <c:overlap val="-25"/>
-        <c:axId val="195318528"/>
-        <c:axId val="195320064"/>
+        <c:axId val="185481088"/>
+        <c:axId val="185482624"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="195318528"/>
+        <c:axId val="185481088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="195320064"/>
+        <c:crossAx val="185482624"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="195320064"/>
+        <c:axId val="185482624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1228,7 +1228,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="195318528"/>
+        <c:crossAx val="185481088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1237,7 +1237,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000289" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000289" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.750000000000003" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000003" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1554,8 +1554,8 @@
         </c:ser>
         <c:gapWidth val="75"/>
         <c:overlap val="-25"/>
-        <c:axId val="195491328"/>
-        <c:axId val="195489792"/>
+        <c:axId val="185593856"/>
+        <c:axId val="185592064"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -1802,11 +1802,11 @@
           <c:smooth val="1"/>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="195478272"/>
-        <c:axId val="195479808"/>
+        <c:axId val="185580544"/>
+        <c:axId val="185590528"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="195478272"/>
+        <c:axId val="185580544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1814,13 +1814,13 @@
         <c:numFmt formatCode="d/m" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="195479808"/>
+        <c:crossAx val="185590528"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="195479808"/>
+        <c:axId val="185590528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1834,24 +1834,24 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="195478272"/>
+        <c:crossAx val="185580544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="195489792"/>
+        <c:axId val="185592064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="r"/>
         <c:numFmt formatCode="#,##0" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="195491328"/>
+        <c:crossAx val="185593856"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:dateAx>
-        <c:axId val="195491328"/>
+        <c:axId val="185593856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1859,7 +1859,7 @@
         <c:axPos val="b"/>
         <c:numFmt formatCode="dd\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="195489792"/>
+        <c:crossAx val="185592064"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
@@ -1874,7 +1874,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000266" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000266" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000278" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000278" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
   <c:userShapes r:id="rId1"/>
@@ -2185,25 +2185,25 @@
         </c:ser>
         <c:gapWidth val="75"/>
         <c:overlap val="-25"/>
-        <c:axId val="195585536"/>
-        <c:axId val="195587072"/>
+        <c:axId val="185823232"/>
+        <c:axId val="185824768"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="195585536"/>
+        <c:axId val="185823232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="195587072"/>
+        <c:crossAx val="185824768"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="195587072"/>
+        <c:axId val="185824768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2217,7 +2217,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="195585536"/>
+        <c:crossAx val="185823232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2226,7 +2226,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000244" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000244" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000255" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000255" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2533,25 +2533,25 @@
         </c:ser>
         <c:gapWidth val="75"/>
         <c:overlap val="-25"/>
-        <c:axId val="195615360"/>
-        <c:axId val="196157824"/>
+        <c:axId val="185853056"/>
+        <c:axId val="185854592"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="195615360"/>
+        <c:axId val="185853056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="196157824"/>
+        <c:crossAx val="185854592"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="196157824"/>
+        <c:axId val="185854592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2565,7 +2565,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="195615360"/>
+        <c:crossAx val="185853056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2574,7 +2574,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000266" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000266" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000278" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000278" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2891,8 +2891,8 @@
         </c:ser>
         <c:gapWidth val="75"/>
         <c:overlap val="-25"/>
-        <c:axId val="196189184"/>
-        <c:axId val="196187648"/>
+        <c:axId val="185694848"/>
+        <c:axId val="185693312"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -3139,11 +3139,11 @@
           <c:smooth val="1"/>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="196180224"/>
-        <c:axId val="196186112"/>
+        <c:axId val="185685888"/>
+        <c:axId val="185687424"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="196180224"/>
+        <c:axId val="185685888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3151,13 +3151,13 @@
         <c:numFmt formatCode="d/m" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="196186112"/>
+        <c:crossAx val="185687424"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="196186112"/>
+        <c:axId val="185687424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3171,24 +3171,24 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="196180224"/>
+        <c:crossAx val="185685888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="196187648"/>
+        <c:axId val="185693312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="r"/>
         <c:numFmt formatCode="#,##0" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="196189184"/>
+        <c:crossAx val="185694848"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:dateAx>
-        <c:axId val="196189184"/>
+        <c:axId val="185694848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3196,7 +3196,7 @@
         <c:axPos val="b"/>
         <c:numFmt formatCode="dd\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="196187648"/>
+        <c:crossAx val="185693312"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
@@ -3211,7 +3211,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000266" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000266" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000278" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000278" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3521,25 +3521,25 @@
         </c:ser>
         <c:gapWidth val="75"/>
         <c:overlap val="-25"/>
-        <c:axId val="196205568"/>
-        <c:axId val="196227840"/>
+        <c:axId val="185723520"/>
+        <c:axId val="185741696"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="196205568"/>
+        <c:axId val="185723520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="196227840"/>
+        <c:crossAx val="185741696"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="196227840"/>
+        <c:axId val="185741696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3553,7 +3553,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="196205568"/>
+        <c:crossAx val="185723520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3562,7 +3562,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000289" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000289" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.750000000000003" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000003" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3788,27 +3788,29 @@
         </c:ser>
         <c:gapWidth val="75"/>
         <c:overlap val="-25"/>
-        <c:axId val="193686912"/>
-        <c:axId val="193623168"/>
+        <c:axId val="183096064"/>
+        <c:axId val="183097600"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="193686912"/>
+        <c:axId val="183096064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="193623168"/>
+        <c:crossAx val="183097600"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="193623168"/>
+        <c:axId val="183097600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="12000"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:majorGridlines/>
@@ -3820,7 +3822,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="193686912"/>
+        <c:crossAx val="183096064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3829,7 +3831,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000222" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000222" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000233" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000233" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4058,25 +4060,25 @@
         </c:ser>
         <c:gapWidth val="75"/>
         <c:overlap val="-25"/>
-        <c:axId val="193732992"/>
-        <c:axId val="193734528"/>
+        <c:axId val="184825344"/>
+        <c:axId val="184826880"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="193732992"/>
+        <c:axId val="184825344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="193734528"/>
+        <c:crossAx val="184826880"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="193734528"/>
+        <c:axId val="184826880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4090,7 +4092,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="193732992"/>
+        <c:crossAx val="184825344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4099,7 +4101,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000244" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000244" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000255" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000255" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4332,8 +4334,8 @@
         </c:ser>
         <c:gapWidth val="75"/>
         <c:overlap val="-25"/>
-        <c:axId val="194057728"/>
-        <c:axId val="194056192"/>
+        <c:axId val="184883840"/>
+        <c:axId val="184882304"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -4490,11 +4492,11 @@
           <c:smooth val="1"/>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="193786624"/>
-        <c:axId val="193788160"/>
+        <c:axId val="184870784"/>
+        <c:axId val="184872320"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="193786624"/>
+        <c:axId val="184870784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4512,13 +4514,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="193788160"/>
+        <c:crossAx val="184872320"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="193788160"/>
+        <c:axId val="184872320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4532,24 +4534,24 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="193786624"/>
+        <c:crossAx val="184870784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="194056192"/>
+        <c:axId val="184882304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="r"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="194057728"/>
+        <c:crossAx val="184883840"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:dateAx>
-        <c:axId val="194057728"/>
+        <c:axId val="184883840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4557,7 +4559,7 @@
         <c:axPos val="b"/>
         <c:numFmt formatCode="dd\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="194056192"/>
+        <c:crossAx val="184882304"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
@@ -4572,7 +4574,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000244" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000244" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000255" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000255" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4798,25 +4800,25 @@
         </c:ser>
         <c:gapWidth val="75"/>
         <c:overlap val="-25"/>
-        <c:axId val="194081152"/>
-        <c:axId val="194082688"/>
+        <c:axId val="184894976"/>
+        <c:axId val="184896512"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="194081152"/>
+        <c:axId val="184894976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="194082688"/>
+        <c:crossAx val="184896512"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="194082688"/>
+        <c:axId val="184896512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4830,7 +4832,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="194081152"/>
+        <c:crossAx val="184894976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4839,7 +4841,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000266" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000266" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000278" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000278" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -5102,8 +5104,8 @@
         </c:ser>
         <c:gapWidth val="75"/>
         <c:overlap val="-25"/>
-        <c:axId val="195213184"/>
-        <c:axId val="195211648"/>
+        <c:axId val="185170944"/>
+        <c:axId val="185169408"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -5299,11 +5301,11 @@
           <c:smooth val="1"/>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="195204224"/>
-        <c:axId val="195205760"/>
+        <c:axId val="185161984"/>
+        <c:axId val="185167872"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="195204224"/>
+        <c:axId val="185161984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5321,13 +5323,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="195205760"/>
+        <c:crossAx val="185167872"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="195205760"/>
+        <c:axId val="185167872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5341,24 +5343,24 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="195204224"/>
+        <c:crossAx val="185161984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="195211648"/>
+        <c:axId val="185169408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="r"/>
         <c:numFmt formatCode="#,##0" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="195213184"/>
+        <c:crossAx val="185170944"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:dateAx>
-        <c:axId val="195213184"/>
+        <c:axId val="185170944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5366,7 +5368,7 @@
         <c:axPos val="b"/>
         <c:numFmt formatCode="dd\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="195211648"/>
+        <c:crossAx val="185169408"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
@@ -5381,7 +5383,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000266" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000266" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000278" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000278" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
   <c:userShapes r:id="rId1"/>
@@ -5638,25 +5640,25 @@
         </c:ser>
         <c:gapWidth val="75"/>
         <c:overlap val="-25"/>
-        <c:axId val="195222528"/>
-        <c:axId val="195405696"/>
+        <c:axId val="185361152"/>
+        <c:axId val="185363456"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="195222528"/>
+        <c:axId val="185361152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="195405696"/>
+        <c:crossAx val="185363456"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="195405696"/>
+        <c:axId val="185363456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5670,7 +5672,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="195222528"/>
+        <c:crossAx val="185361152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5679,7 +5681,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000244" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000244" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000255" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000255" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -5935,25 +5937,25 @@
         </c:ser>
         <c:gapWidth val="75"/>
         <c:overlap val="-25"/>
-        <c:axId val="194867968"/>
-        <c:axId val="194869504"/>
+        <c:axId val="185382784"/>
+        <c:axId val="185384320"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="194867968"/>
+        <c:axId val="185382784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="194869504"/>
+        <c:crossAx val="185384320"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="194869504"/>
+        <c:axId val="185384320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5967,7 +5969,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="194867968"/>
+        <c:crossAx val="185382784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5976,7 +5978,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000266" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000266" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000278" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000278" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -6209,8 +6211,8 @@
         </c:ser>
         <c:gapWidth val="75"/>
         <c:overlap val="-25"/>
-        <c:axId val="195299584"/>
-        <c:axId val="195298048"/>
+        <c:axId val="185458048"/>
+        <c:axId val="185456512"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -6388,11 +6390,11 @@
           <c:smooth val="1"/>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="194848256"/>
-        <c:axId val="194849792"/>
+        <c:axId val="185440896"/>
+        <c:axId val="185454976"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="194848256"/>
+        <c:axId val="185440896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6410,13 +6412,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="194849792"/>
+        <c:crossAx val="185454976"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="194849792"/>
+        <c:axId val="185454976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6430,24 +6432,24 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="194848256"/>
+        <c:crossAx val="185440896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="195298048"/>
+        <c:axId val="185456512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="r"/>
         <c:numFmt formatCode="#,##0" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="195299584"/>
+        <c:crossAx val="185458048"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:dateAx>
-        <c:axId val="195299584"/>
+        <c:axId val="185458048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6455,7 +6457,7 @@
         <c:axPos val="b"/>
         <c:numFmt formatCode="dd\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="195298048"/>
+        <c:crossAx val="185456512"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
@@ -6470,7 +6472,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000266" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000266" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000278" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000278" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -7545,11 +7547,11 @@
       <selection activeCell="E117" sqref="E117"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" style="21" customWidth="1"/>
-    <col min="3" max="6" width="14.7109375" style="2" customWidth="1"/>
+    <col min="1" max="1" width="14.6640625" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" style="21" customWidth="1"/>
+    <col min="3" max="6" width="14.6640625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="7" customFormat="1">
@@ -9409,22 +9411,22 @@
       <selection activeCell="AE47" sqref="AE47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" style="6" customWidth="1"/>
-    <col min="2" max="2" width="11.28515625" style="13" customWidth="1"/>
-    <col min="3" max="4" width="10.7109375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" style="11" customWidth="1"/>
-    <col min="6" max="6" width="1.28515625" style="2" customWidth="1"/>
-    <col min="7" max="8" width="10.7109375" style="2" customWidth="1"/>
-    <col min="9" max="9" width="10.7109375" style="1" customWidth="1"/>
-    <col min="10" max="10" width="7.7109375" style="16" customWidth="1"/>
-    <col min="11" max="11" width="1.140625" customWidth="1"/>
-    <col min="15" max="15" width="7.7109375" style="19" customWidth="1"/>
-    <col min="16" max="16" width="3.7109375" customWidth="1"/>
+    <col min="1" max="1" width="10.6640625" style="6" customWidth="1"/>
+    <col min="2" max="2" width="11.33203125" style="13" customWidth="1"/>
+    <col min="3" max="4" width="10.6640625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="10.6640625" style="11" customWidth="1"/>
+    <col min="6" max="6" width="1.33203125" style="2" customWidth="1"/>
+    <col min="7" max="8" width="10.6640625" style="2" customWidth="1"/>
+    <col min="9" max="9" width="10.6640625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="7.6640625" style="16" customWidth="1"/>
+    <col min="11" max="11" width="1.109375" customWidth="1"/>
+    <col min="15" max="15" width="7.6640625" style="19" customWidth="1"/>
+    <col min="16" max="16" width="3.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="28.5">
+    <row r="1" spans="1:16" ht="28.8">
       <c r="A1" s="23" t="s">
         <v>9</v>
       </c>
@@ -9446,7 +9448,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="15.75" thickBot="1">
+    <row r="3" spans="1:16" ht="15" thickBot="1">
       <c r="B3" s="14" t="s">
         <v>13</v>
       </c>
@@ -10810,26 +10812,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:P38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M34" sqref="M34:O35"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" style="6" customWidth="1"/>
-    <col min="2" max="2" width="11.28515625" style="13" customWidth="1"/>
-    <col min="3" max="4" width="10.7109375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" style="11" customWidth="1"/>
-    <col min="6" max="6" width="1.28515625" style="2" customWidth="1"/>
-    <col min="7" max="8" width="10.7109375" style="2" customWidth="1"/>
-    <col min="9" max="9" width="10.7109375" style="1" customWidth="1"/>
-    <col min="10" max="10" width="7.7109375" style="16" customWidth="1"/>
-    <col min="11" max="11" width="1.140625" customWidth="1"/>
-    <col min="15" max="15" width="7.7109375" style="19" customWidth="1"/>
-    <col min="16" max="16" width="3.7109375" customWidth="1"/>
+    <col min="1" max="1" width="10.6640625" style="6" customWidth="1"/>
+    <col min="2" max="2" width="11.33203125" style="13" customWidth="1"/>
+    <col min="3" max="4" width="10.6640625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="10.6640625" style="11" customWidth="1"/>
+    <col min="6" max="6" width="1.33203125" style="2" customWidth="1"/>
+    <col min="7" max="8" width="10.6640625" style="2" customWidth="1"/>
+    <col min="9" max="9" width="10.6640625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="7.6640625" style="16" customWidth="1"/>
+    <col min="11" max="11" width="1.109375" customWidth="1"/>
+    <col min="15" max="15" width="7.6640625" style="19" customWidth="1"/>
+    <col min="16" max="16" width="3.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="28.5">
+    <row r="1" spans="1:16" ht="28.8">
       <c r="A1" s="23" t="s">
         <v>10</v>
       </c>
@@ -10851,7 +10853,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="15.75" thickBot="1">
+    <row r="3" spans="1:16" ht="15" thickBot="1">
       <c r="B3" s="14" t="s">
         <v>13</v>
       </c>
@@ -12454,27 +12456,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:P47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="AH31" sqref="AH31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" style="6" customWidth="1"/>
-    <col min="2" max="2" width="11.28515625" style="13" customWidth="1"/>
-    <col min="3" max="4" width="10.7109375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" style="11" customWidth="1"/>
-    <col min="6" max="6" width="1.28515625" style="2" customWidth="1"/>
-    <col min="7" max="8" width="10.7109375" style="2" customWidth="1"/>
-    <col min="9" max="9" width="10.7109375" style="1" customWidth="1"/>
-    <col min="10" max="10" width="7.7109375" style="16" customWidth="1"/>
-    <col min="11" max="11" width="1.140625" customWidth="1"/>
-    <col min="12" max="12" width="8.85546875" style="2"/>
-    <col min="15" max="15" width="7.7109375" style="19" customWidth="1"/>
-    <col min="16" max="16" width="3.7109375" customWidth="1"/>
+    <col min="1" max="1" width="10.6640625" style="6" customWidth="1"/>
+    <col min="2" max="2" width="11.33203125" style="13" customWidth="1"/>
+    <col min="3" max="4" width="10.6640625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="10.6640625" style="11" customWidth="1"/>
+    <col min="6" max="6" width="1.33203125" style="2" customWidth="1"/>
+    <col min="7" max="8" width="10.6640625" style="2" customWidth="1"/>
+    <col min="9" max="9" width="10.6640625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="7.6640625" style="16" customWidth="1"/>
+    <col min="11" max="11" width="1.109375" customWidth="1"/>
+    <col min="12" max="12" width="8.88671875" style="2"/>
+    <col min="15" max="15" width="7.6640625" style="19" customWidth="1"/>
+    <col min="16" max="16" width="3.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="28.5">
+    <row r="1" spans="1:16" ht="28.8">
       <c r="A1" s="23" t="s">
         <v>16</v>
       </c>
@@ -12496,7 +12498,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="15.75" thickBot="1">
+    <row r="3" spans="1:16" ht="15" thickBot="1">
       <c r="B3" s="14" t="s">
         <v>13</v>
       </c>
@@ -14567,7 +14569,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -14579,7 +14581,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>